<commit_message>
Commands of Branch entered please check
</commit_message>
<xml_diff>
--- a/Git progress.xlsx
+++ b/Git progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavir\OneDrive\Desktop\New folder\Gitpractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE85030-B548-495D-90B2-A5CE0F0C7C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF760E7B-DD2B-47FB-8909-F7F5D28651F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2DC466C-4B68-4FCD-988F-760D626F941A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Requirement/issue</t>
   </si>
@@ -74,6 +74,82 @@
       </rPr>
       <t>(git clone https://github.com/Narra-Srinivas/Gitpractice.git)</t>
     </r>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>To create a new branch</t>
+  </si>
+  <si>
+    <t>Branch command to be used</t>
+  </si>
+  <si>
+    <t>git branch 'branch_name'</t>
+  </si>
+  <si>
+    <t>switch/checkout</t>
+  </si>
+  <si>
+    <t>git switch 'branch_name'/ git checkout 'branch_name'</t>
+  </si>
+  <si>
+    <t>To change to other branch</t>
+  </si>
+  <si>
+    <t>To create a new branch and change to it at once</t>
+  </si>
+  <si>
+    <t>1. git switch -c 'branch_name' 
+2.git checkout -b 'branch_name'</t>
+  </si>
+  <si>
+    <t>To list branches that are currently in working mode</t>
+  </si>
+  <si>
+    <t>can be done either using switch -c and checkout -b</t>
+  </si>
+  <si>
+    <t>use branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git branch </t>
+  </si>
+  <si>
+    <t>To list all the branches</t>
+  </si>
+  <si>
+    <t>use branch -a</t>
+  </si>
+  <si>
+    <t>git branch -a</t>
+  </si>
+  <si>
+    <t>To rename the branches</t>
+  </si>
+  <si>
+    <t>branch -m</t>
+  </si>
+  <si>
+    <t>git branch -m 'old branch name' 'new branch name'</t>
+  </si>
+  <si>
+    <t>To delete a particular branch</t>
+  </si>
+  <si>
+    <t>branch -d</t>
+  </si>
+  <si>
+    <t>git branch -d 'branch name'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do forceful deletion </t>
+  </si>
+  <si>
+    <t>branch -D</t>
+  </si>
+  <si>
+    <t>git branch -D 'branch name'</t>
   </si>
 </sst>
 </file>
@@ -129,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -140,8 +216,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA861CEB-41D1-42AE-A5DC-C978A8FB9082}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -526,11 +611,98 @@
         <v>50</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit and add commands are also added
</commit_message>
<xml_diff>
--- a/Git progress.xlsx
+++ b/Git progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavir\OneDrive\Desktop\New folder\Gitpractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF760E7B-DD2B-47FB-8909-F7F5D28651F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C943AD8-E971-4D03-A8B0-EE3C8F2CC1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2DC466C-4B68-4FCD-988F-760D626F941A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Requirement/issue</t>
   </si>
@@ -104,9 +104,6 @@
 2.git checkout -b 'branch_name'</t>
   </si>
   <si>
-    <t>To list branches that are currently in working mode</t>
-  </si>
-  <si>
     <t>can be done either using switch -c and checkout -b</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t xml:space="preserve">git branch </t>
   </si>
   <si>
-    <t>To list all the branches</t>
-  </si>
-  <si>
     <t>use branch -a</t>
   </si>
   <si>
@@ -150,6 +144,48 @@
   </si>
   <si>
     <t>git branch -D 'branch name'</t>
+  </si>
+  <si>
+    <t>To list branches that are currently in working  directory</t>
+  </si>
+  <si>
+    <t>To list all the branches (local &amp; remote)</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>To add the work done in the working directory</t>
+  </si>
+  <si>
+    <t>use add</t>
+  </si>
+  <si>
+    <t>git add 'File name'</t>
+  </si>
+  <si>
+    <t>To add all the files</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add </t>
+  </si>
+  <si>
+    <t>To commit the work done</t>
+  </si>
+  <si>
+    <t>commit -m</t>
+  </si>
+  <si>
+    <t>git commit -m 'Message to be given'</t>
+  </si>
+  <si>
+    <t>git commit -m 'Subject' -m 'Description'</t>
   </si>
 </sst>
 </file>
@@ -562,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA861CEB-41D1-42AE-A5DC-C978A8FB9082}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C20" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -605,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>50</v>
@@ -643,7 +679,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>16</v>
@@ -651,60 +687,109 @@
     </row>
     <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>